<commit_message>
Updated data from WRI for HK EPS 2.0 update
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant.xlsx
+++ b/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoHIbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mengpin.ge\World Resources Institute\TRAC City - HK 2050 is now\EPS HK 2.0\eps-2.0.0-us-wipF\InputData\add-outputs\SCoHIbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_C64E0802DF4F489855998562BBAAF410B147BB96" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19140" windowHeight="6435"/>
+    <workbookView xWindow="405" yWindow="0" windowWidth="17355" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,15 @@
     <sheet name="SCoHIbP-indst" sheetId="9" r:id="rId7"/>
     <sheet name="SCoHIbP-LULUCF" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -289,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -477,14 +486,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,6 +584,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -610,6 +636,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -785,10 +828,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -950,7 +995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1140,7 +1185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5172,7 +5217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -7140,7 +7185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9108,7 +9153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -11076,7 +11121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13045,7 +13090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -15013,6 +15058,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15246,32 +15309,48 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91F9C728-182A-4DD9-BAC8-30EE24809206}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F299B580-03AC-4A2B-97DE-D1E6FD2FE7C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CDC76DE-FAD9-4B8B-9EE3-B689859529E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CDC76DE-FAD9-4B8B-9EE3-B689859529E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F299B580-03AC-4A2B-97DE-D1E6FD2FE7C5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91F9C728-182A-4DD9-BAC8-30EE24809206}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to 2.1.1 and CSV export tool run.
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant.xlsx
+++ b/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mengpin.ge\World Resources Institute\TRAC City - HK 2050 is now\eps-1.4.3-hk-wipB\eps-1.4.3-hk-wipB\InputData\add-outputs\SCoHIbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-hongkong\InputData\add-outputs\SCoHIbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_1EA5BA938449F181D9695CECA5550F01C728FAD2" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{B78FF202-A604-4A20-A7DC-936DC8901BBF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,8 +17,9 @@
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
     <sheet name="SCoHIbP-transportation" sheetId="4" r:id="rId4"/>
     <sheet name="SCoHIbP-elec-distheat" sheetId="5" r:id="rId5"/>
-    <sheet name="SCoHIbP-bldgs-indst" sheetId="6" r:id="rId6"/>
-    <sheet name="SCoHIbP-LULUCF" sheetId="7" r:id="rId7"/>
+    <sheet name="SCoHIbP-bldgs" sheetId="6" r:id="rId6"/>
+    <sheet name="SCoHIbP-indst" sheetId="8" r:id="rId7"/>
+    <sheet name="SCoHIbP-LULUCF" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="86">
   <si>
     <t>SCoHIbP Social Cost of Health Impacts by Pollutant</t>
   </si>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -476,14 +476,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -574,23 +574,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -626,23 +609,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,25 +784,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -844,157 +810,157 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="15"/>
       <c r="B4" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="15"/>
       <c r="B5" s="2">
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="15"/>
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="15"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="15">
         <v>1.141</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="15"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="15"/>
       <c r="B39" s="18" t="s">
         <v>28</v>
@@ -1002,7 +968,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{834DBD59-10B1-4AE6-A3A8-02185DFC478C}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -1010,19 +976,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="13" width="14.42578125" customWidth="1"/>
+    <col min="2" max="13" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1039,7 +1005,7 @@
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1080,7 +1046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>2015</v>
       </c>
@@ -1121,7 +1087,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>2020</v>
       </c>
@@ -1162,7 +1128,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>2030</v>
       </c>
@@ -1209,24 +1175,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M160"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5703125" customWidth="1"/>
-    <col min="11" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="5" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.59765625" customWidth="1"/>
+    <col min="11" max="12" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>43</v>
       </c>
@@ -1236,7 +1202,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>44</v>
       </c>
@@ -1246,7 +1212,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
@@ -1256,7 +1222,7 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>46</v>
       </c>
@@ -1266,7 +1232,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>47</v>
       </c>
@@ -1276,7 +1242,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>48</v>
       </c>
@@ -1286,7 +1252,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>49</v>
       </c>
@@ -1296,7 +1262,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>50</v>
       </c>
@@ -1306,7 +1272,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1292,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>2015</v>
       </c>
@@ -1351,7 +1317,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>2020</v>
       </c>
@@ -1376,7 +1342,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>2030</v>
       </c>
@@ -1401,7 +1367,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
@@ -1411,7 +1377,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>2015</v>
       </c>
@@ -1456,7 +1422,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>2020</v>
       </c>
@@ -1481,7 +1447,7 @@
         <v>19000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <v>2030</v>
       </c>
@@ -1506,7 +1472,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>56</v>
       </c>
@@ -1516,7 +1482,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1536,7 +1502,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>2015</v>
       </c>
@@ -1561,7 +1527,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>2020</v>
       </c>
@@ -1586,7 +1552,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>2030</v>
       </c>
@@ -1611,7 +1577,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1619,7 +1585,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
@@ -1629,7 +1595,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1649,7 +1615,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <v>2015</v>
       </c>
@@ -1674,7 +1640,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <v>2020</v>
       </c>
@@ -1699,7 +1665,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <v>2030</v>
       </c>
@@ -1724,7 +1690,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>58</v>
       </c>
@@ -1741,7 +1707,7 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>59</v>
       </c>
@@ -1758,7 +1724,7 @@
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>60</v>
       </c>
@@ -1775,7 +1741,7 @@
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>61</v>
       </c>
@@ -1792,7 +1758,7 @@
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
         <v>62</v>
       </c>
@@ -1809,7 +1775,7 @@
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -1826,7 +1792,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>30</v>
       </c>
@@ -1867,7 +1833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="6">
         <v>2015</v>
       </c>
@@ -1912,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="6">
         <v>2020</v>
       </c>
@@ -1957,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="6">
         <v>2030</v>
       </c>
@@ -2002,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>55</v>
       </c>
@@ -2019,7 +1985,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -2060,7 +2026,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" s="6">
         <v>2015</v>
       </c>
@@ -2105,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" s="6">
         <v>2020</v>
       </c>
@@ -2150,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" s="6">
         <v>2030</v>
       </c>
@@ -2195,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>56</v>
       </c>
@@ -2212,7 +2178,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -2253,7 +2219,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" s="6">
         <v>2015</v>
       </c>
@@ -2298,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" s="6">
         <v>2020</v>
       </c>
@@ -2343,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" s="6">
         <v>2030</v>
       </c>
@@ -2388,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" s="6"/>
       <c r="B57" s="15"/>
       <c r="C57" s="5"/>
@@ -2403,7 +2369,7 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
         <v>57</v>
       </c>
@@ -2420,7 +2386,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>30</v>
       </c>
@@ -2461,7 +2427,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60" s="6">
         <v>2015</v>
       </c>
@@ -2506,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" s="6">
         <v>2020</v>
       </c>
@@ -2551,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" s="6">
         <v>2030</v>
       </c>
@@ -2596,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64" s="15" t="s">
         <v>72</v>
       </c>
@@ -2613,7 +2579,7 @@
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>50</v>
       </c>
@@ -2630,7 +2596,7 @@
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>30</v>
       </c>
@@ -2671,7 +2637,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68" s="6">
         <v>2015</v>
       </c>
@@ -2724,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69" s="6">
         <v>2020</v>
       </c>
@@ -2777,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70" s="6">
         <v>2030</v>
       </c>
@@ -2830,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" s="9" t="s">
         <v>55</v>
       </c>
@@ -2847,7 +2813,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>30</v>
       </c>
@@ -2888,7 +2854,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A74" s="6">
         <v>2015</v>
       </c>
@@ -2941,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="6">
         <v>2020</v>
       </c>
@@ -2994,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76" s="6">
         <v>2030</v>
       </c>
@@ -3047,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78" s="9" t="s">
         <v>56</v>
       </c>
@@ -3064,7 +3030,7 @@
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>30</v>
       </c>
@@ -3105,7 +3071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80" s="6">
         <v>2015</v>
       </c>
@@ -3158,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81" s="6">
         <v>2020</v>
       </c>
@@ -3211,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A82" s="6">
         <v>2030</v>
       </c>
@@ -3264,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A83" s="6"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -3279,7 +3245,7 @@
       <c r="L83" s="5"/>
       <c r="M83" s="5"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>57</v>
       </c>
@@ -3296,7 +3262,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>30</v>
       </c>
@@ -3337,7 +3303,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86" s="6">
         <v>2015</v>
       </c>
@@ -3390,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A87" s="6">
         <v>2020</v>
       </c>
@@ -3443,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88" s="6">
         <v>2030</v>
       </c>
@@ -3496,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A90" s="15" t="s">
         <v>73</v>
       </c>
@@ -3513,7 +3479,7 @@
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>74</v>
       </c>
@@ -3533,7 +3499,7 @@
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
     </row>
-    <row r="94" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A94" s="9" t="s">
         <v>50</v>
       </c>
@@ -3550,7 +3516,7 @@
       <c r="L94" s="10"/>
       <c r="M94" s="10"/>
     </row>
-    <row r="95" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>30</v>
       </c>
@@ -3591,7 +3557,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A96" s="6">
         <v>2015</v>
       </c>
@@ -3644,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A97" s="6">
         <v>2020</v>
       </c>
@@ -3697,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A98" s="6">
         <v>2030</v>
       </c>
@@ -3750,8 +3716,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="100" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A100" s="9" t="s">
         <v>55</v>
       </c>
@@ -3768,7 +3734,7 @@
       <c r="L100" s="10"/>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>30</v>
       </c>
@@ -3809,7 +3775,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A102" s="6">
         <v>2015</v>
       </c>
@@ -3862,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A103" s="6">
         <v>2020</v>
       </c>
@@ -3915,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A104" s="6">
         <v>2030</v>
       </c>
@@ -3968,8 +3934,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="106" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="9" t="s">
         <v>56</v>
       </c>
@@ -3986,7 +3952,7 @@
       <c r="L106" s="10"/>
       <c r="M106" s="10"/>
     </row>
-    <row r="107" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>30</v>
       </c>
@@ -4027,7 +3993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A108" s="6">
         <v>2015</v>
       </c>
@@ -4080,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A109" s="6">
         <v>2020</v>
       </c>
@@ -4133,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A110" s="6">
         <v>2030</v>
       </c>
@@ -4186,7 +4152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A111" s="6"/>
       <c r="B111" s="5"/>
       <c r="C111" s="12"/>
@@ -4201,7 +4167,7 @@
       <c r="L111" s="5"/>
       <c r="M111" s="5"/>
     </row>
-    <row r="112" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A112" s="13" t="s">
         <v>57</v>
       </c>
@@ -4218,7 +4184,7 @@
       <c r="L112" s="10"/>
       <c r="M112" s="10"/>
     </row>
-    <row r="113" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>30</v>
       </c>
@@ -4259,7 +4225,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A114" s="6">
         <v>2015</v>
       </c>
@@ -4312,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A115" s="6">
         <v>2020</v>
       </c>
@@ -4365,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A116" s="6">
         <v>2030</v>
       </c>
@@ -4418,74 +4384,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="118" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="119" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A120" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A121" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="123" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A123" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="124" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A124" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A125" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="126" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="127" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A127" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A128" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="129" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="130" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A131" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="133" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A134" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A136" s="9" t="s">
         <v>50</v>
       </c>
@@ -4502,7 +4468,7 @@
       <c r="L136" s="10"/>
       <c r="M136" s="10"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
         <v>30</v>
       </c>
@@ -4543,7 +4509,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A138" s="6">
         <v>2015</v>
       </c>
@@ -4596,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A139" s="6">
         <v>2020</v>
       </c>
@@ -4649,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A140" s="6">
         <v>2030</v>
       </c>
@@ -4702,7 +4668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A142" s="9" t="s">
         <v>55</v>
       </c>
@@ -4719,7 +4685,7 @@
       <c r="L142" s="10"/>
       <c r="M142" s="10"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A143" s="1" t="s">
         <v>30</v>
       </c>
@@ -4760,7 +4726,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A144" s="6">
         <v>2015</v>
       </c>
@@ -4813,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A145" s="6">
         <v>2020</v>
       </c>
@@ -4866,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A146" s="6">
         <v>2030</v>
       </c>
@@ -4919,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A148" s="9" t="s">
         <v>56</v>
       </c>
@@ -4936,7 +4902,7 @@
       <c r="L148" s="10"/>
       <c r="M148" s="10"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
         <v>30</v>
       </c>
@@ -4977,7 +4943,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A150" s="6">
         <v>2015</v>
       </c>
@@ -5030,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A151" s="6">
         <v>2020</v>
       </c>
@@ -5083,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A152" s="6">
         <v>2030</v>
       </c>
@@ -5136,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A153" s="6"/>
       <c r="B153" s="5"/>
       <c r="C153" s="12"/>
@@ -5151,7 +5117,7 @@
       <c r="L153" s="5"/>
       <c r="M153" s="5"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A154" s="13" t="s">
         <v>57</v>
       </c>
@@ -5168,7 +5134,7 @@
       <c r="L154" s="10"/>
       <c r="M154" s="10"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
         <v>30</v>
       </c>
@@ -5209,7 +5175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A156" s="6">
         <v>2015</v>
       </c>
@@ -5262,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A157" s="6">
         <v>2020</v>
       </c>
@@ -5315,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A158" s="6">
         <v>2030</v>
       </c>
@@ -5368,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A160" s="15" t="s">
         <v>85</v>
       </c>
@@ -5392,7 +5358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -5402,9 +5368,9 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -5445,7 +5411,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="15">
         <v>2015</v>
       </c>
@@ -5486,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="15">
         <v>2016</v>
       </c>
@@ -5527,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>2017</v>
       </c>
@@ -5568,7 +5534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="15">
         <v>2018</v>
       </c>
@@ -5609,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="15">
         <v>2019</v>
       </c>
@@ -5650,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="15">
         <v>2020</v>
       </c>
@@ -5691,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>2021</v>
       </c>
@@ -5732,7 +5698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15">
         <v>2022</v>
       </c>
@@ -5773,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>2023</v>
       </c>
@@ -5814,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>2024</v>
       </c>
@@ -5855,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>2025</v>
       </c>
@@ -5896,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>2026</v>
       </c>
@@ -5937,7 +5903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>2027</v>
       </c>
@@ -5978,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>2028</v>
       </c>
@@ -6019,7 +5985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>2029</v>
       </c>
@@ -6060,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>2030</v>
       </c>
@@ -6101,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>2031</v>
       </c>
@@ -6142,7 +6108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>2032</v>
       </c>
@@ -6183,7 +6149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15">
         <v>2033</v>
       </c>
@@ -6224,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15">
         <v>2034</v>
       </c>
@@ -6265,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="15">
         <v>2035</v>
       </c>
@@ -6306,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15">
         <v>2036</v>
       </c>
@@ -6347,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15">
         <v>2037</v>
       </c>
@@ -6388,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="15">
         <v>2038</v>
       </c>
@@ -6429,7 +6395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15">
         <v>2039</v>
       </c>
@@ -6470,7 +6436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15">
         <v>2040</v>
       </c>
@@ -6511,7 +6477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15">
         <v>2041</v>
       </c>
@@ -6552,7 +6518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15">
         <v>2042</v>
       </c>
@@ -6593,7 +6559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15">
         <v>2043</v>
       </c>
@@ -6634,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15">
         <v>2044</v>
       </c>
@@ -6675,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="15">
         <v>2045</v>
       </c>
@@ -6716,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15">
         <v>2046</v>
       </c>
@@ -6757,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15">
         <v>2047</v>
       </c>
@@ -6798,7 +6764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15">
         <v>2048</v>
       </c>
@@ -6839,7 +6805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15">
         <v>2049</v>
       </c>
@@ -6880,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15">
         <v>2050</v>
       </c>
@@ -6927,7 +6893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6937,9 +6903,9 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -6980,7 +6946,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="15">
         <v>2015</v>
       </c>
@@ -7021,7 +6987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="15">
         <v>2016</v>
       </c>
@@ -7062,7 +7028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>2017</v>
       </c>
@@ -7103,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="15">
         <v>2018</v>
       </c>
@@ -7144,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="15">
         <v>2019</v>
       </c>
@@ -7185,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="15">
         <v>2020</v>
       </c>
@@ -7226,7 +7192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>2021</v>
       </c>
@@ -7267,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15">
         <v>2022</v>
       </c>
@@ -7308,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>2023</v>
       </c>
@@ -7349,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>2024</v>
       </c>
@@ -7390,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>2025</v>
       </c>
@@ -7431,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>2026</v>
       </c>
@@ -7472,7 +7438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>2027</v>
       </c>
@@ -7513,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>2028</v>
       </c>
@@ -7554,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>2029</v>
       </c>
@@ -7595,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>2030</v>
       </c>
@@ -7636,7 +7602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>2031</v>
       </c>
@@ -7677,7 +7643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>2032</v>
       </c>
@@ -7718,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15">
         <v>2033</v>
       </c>
@@ -7759,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15">
         <v>2034</v>
       </c>
@@ -7800,7 +7766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="15">
         <v>2035</v>
       </c>
@@ -7841,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15">
         <v>2036</v>
       </c>
@@ -7882,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15">
         <v>2037</v>
       </c>
@@ -7923,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="15">
         <v>2038</v>
       </c>
@@ -7964,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15">
         <v>2039</v>
       </c>
@@ -8005,7 +7971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15">
         <v>2040</v>
       </c>
@@ -8046,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15">
         <v>2041</v>
       </c>
@@ -8087,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15">
         <v>2042</v>
       </c>
@@ -8128,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15">
         <v>2043</v>
       </c>
@@ -8169,7 +8135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15">
         <v>2044</v>
       </c>
@@ -8210,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="15">
         <v>2045</v>
       </c>
@@ -8251,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15">
         <v>2046</v>
       </c>
@@ -8292,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15">
         <v>2047</v>
       </c>
@@ -8333,7 +8299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15">
         <v>2048</v>
       </c>
@@ -8374,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15">
         <v>2049</v>
       </c>
@@ -8415,7 +8381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15">
         <v>2050</v>
       </c>
@@ -8462,7 +8428,1545 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:M37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="9.1328125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="15">
+        <v>2015</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0</v>
+      </c>
+      <c r="K2" s="15">
+        <v>0</v>
+      </c>
+      <c r="L2" s="15">
+        <v>0</v>
+      </c>
+      <c r="M2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="15">
+        <v>2016</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="15">
+        <v>2017</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H4" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="15">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="15">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H6" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0</v>
+      </c>
+      <c r="K6" s="15">
+        <v>0</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="15">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="15">
+        <v>2021</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H8" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0</v>
+      </c>
+      <c r="K8" s="15">
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="15">
+        <v>2022</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0</v>
+      </c>
+      <c r="K9" s="15">
+        <v>0</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="15">
+        <v>2023</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I10" s="15">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
+        <v>0</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="15">
+        <v>2024</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0</v>
+      </c>
+      <c r="G11" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H11" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
+        <v>0</v>
+      </c>
+      <c r="K11" s="15">
+        <v>0</v>
+      </c>
+      <c r="L11" s="15">
+        <v>0</v>
+      </c>
+      <c r="M11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="15">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <v>0</v>
+      </c>
+      <c r="M12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="15">
+        <v>2026</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H13" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="15">
+        <v>2027</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I14" s="15">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0</v>
+      </c>
+      <c r="K14" s="15">
+        <v>0</v>
+      </c>
+      <c r="L14" s="15">
+        <v>0</v>
+      </c>
+      <c r="M14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="15">
+        <v>2028</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="15">
+        <v>2029</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="15">
+        <v>0</v>
+      </c>
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="15">
+        <v>2030</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F17" s="15">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>0</v>
+      </c>
+      <c r="M17" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="15">
+        <v>2031</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0</v>
+      </c>
+      <c r="E18" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="15">
+        <v>2032</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="15">
+        <v>2033</v>
+      </c>
+      <c r="B20" s="15">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0</v>
+      </c>
+      <c r="E20" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F20" s="15">
+        <v>0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H20" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0</v>
+      </c>
+      <c r="J20" s="15">
+        <v>0</v>
+      </c>
+      <c r="K20" s="15">
+        <v>0</v>
+      </c>
+      <c r="L20" s="15">
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="15">
+        <v>2034</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H21" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="15">
+        <v>0</v>
+      </c>
+      <c r="K21" s="15">
+        <v>0</v>
+      </c>
+      <c r="L21" s="15">
+        <v>0</v>
+      </c>
+      <c r="M21" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="15">
+        <v>2035</v>
+      </c>
+      <c r="B22" s="15">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D22" s="15">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H22" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="15">
+        <v>0</v>
+      </c>
+      <c r="K22" s="15">
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
+        <v>0</v>
+      </c>
+      <c r="M22" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="15">
+        <v>2036</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D23" s="15">
+        <v>0</v>
+      </c>
+      <c r="E23" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H23" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0</v>
+      </c>
+      <c r="M23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="15">
+        <v>2037</v>
+      </c>
+      <c r="B24" s="15">
+        <v>0</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D24" s="15">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F24" s="15">
+        <v>0</v>
+      </c>
+      <c r="G24" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H24" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15">
+        <v>0</v>
+      </c>
+      <c r="K24" s="15">
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="15">
+        <v>2038</v>
+      </c>
+      <c r="B25" s="15">
+        <v>0</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D25" s="15">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F25" s="15">
+        <v>0</v>
+      </c>
+      <c r="G25" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H25" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="15">
+        <v>0</v>
+      </c>
+      <c r="K25" s="15">
+        <v>0</v>
+      </c>
+      <c r="L25" s="15">
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A26" s="15">
+        <v>2039</v>
+      </c>
+      <c r="B26" s="15">
+        <v>0</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D26" s="15">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H26" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="15">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A27" s="15">
+        <v>2040</v>
+      </c>
+      <c r="B27" s="15">
+        <v>0</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D27" s="15">
+        <v>0</v>
+      </c>
+      <c r="E27" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F27" s="15">
+        <v>0</v>
+      </c>
+      <c r="G27" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H27" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="15">
+        <v>0</v>
+      </c>
+      <c r="K27" s="15">
+        <v>0</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A28" s="15">
+        <v>2041</v>
+      </c>
+      <c r="B28" s="15">
+        <v>0</v>
+      </c>
+      <c r="C28" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D28" s="15">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F28" s="15">
+        <v>0</v>
+      </c>
+      <c r="G28" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H28" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
+        <v>0</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="15">
+        <v>2042</v>
+      </c>
+      <c r="B29" s="15">
+        <v>0</v>
+      </c>
+      <c r="C29" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0</v>
+      </c>
+      <c r="E29" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F29" s="15">
+        <v>0</v>
+      </c>
+      <c r="G29" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H29" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0</v>
+      </c>
+      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
+        <v>0</v>
+      </c>
+      <c r="M29" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" s="15">
+        <v>2043</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0</v>
+      </c>
+      <c r="C30" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D30" s="15">
+        <v>0</v>
+      </c>
+      <c r="E30" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F30" s="15">
+        <v>0</v>
+      </c>
+      <c r="G30" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H30" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
+        <v>0</v>
+      </c>
+      <c r="M30" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31" s="15">
+        <v>2044</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0</v>
+      </c>
+      <c r="E31" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F31" s="15">
+        <v>0</v>
+      </c>
+      <c r="G31" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H31" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15">
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
+        <v>0</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A32" s="15">
+        <v>2045</v>
+      </c>
+      <c r="B32" s="15">
+        <v>0</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D32" s="15">
+        <v>0</v>
+      </c>
+      <c r="E32" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F32" s="15">
+        <v>0</v>
+      </c>
+      <c r="G32" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H32" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I32" s="15">
+        <v>0</v>
+      </c>
+      <c r="J32" s="15">
+        <v>0</v>
+      </c>
+      <c r="K32" s="15">
+        <v>0</v>
+      </c>
+      <c r="L32" s="15">
+        <v>0</v>
+      </c>
+      <c r="M32" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A33" s="15">
+        <v>2046</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D33" s="15">
+        <v>0</v>
+      </c>
+      <c r="E33" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F33" s="15">
+        <v>0</v>
+      </c>
+      <c r="G33" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H33" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I33" s="15">
+        <v>0</v>
+      </c>
+      <c r="J33" s="15">
+        <v>0</v>
+      </c>
+      <c r="K33" s="15">
+        <v>0</v>
+      </c>
+      <c r="L33" s="15">
+        <v>0</v>
+      </c>
+      <c r="M33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A34" s="15">
+        <v>2047</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0</v>
+      </c>
+      <c r="C34" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D34" s="15">
+        <v>0</v>
+      </c>
+      <c r="E34" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F34" s="15">
+        <v>0</v>
+      </c>
+      <c r="G34" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H34" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I34" s="15">
+        <v>0</v>
+      </c>
+      <c r="J34" s="15">
+        <v>0</v>
+      </c>
+      <c r="K34" s="15">
+        <v>0</v>
+      </c>
+      <c r="L34" s="15">
+        <v>0</v>
+      </c>
+      <c r="M34" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" s="15">
+        <v>2048</v>
+      </c>
+      <c r="B35" s="15">
+        <v>0</v>
+      </c>
+      <c r="C35" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D35" s="15">
+        <v>0</v>
+      </c>
+      <c r="E35" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F35" s="15">
+        <v>0</v>
+      </c>
+      <c r="G35" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H35" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0</v>
+      </c>
+      <c r="J35" s="15">
+        <v>0</v>
+      </c>
+      <c r="K35" s="15">
+        <v>0</v>
+      </c>
+      <c r="L35" s="15">
+        <v>0</v>
+      </c>
+      <c r="M35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="15">
+        <v>2049</v>
+      </c>
+      <c r="B36" s="15">
+        <v>0</v>
+      </c>
+      <c r="C36" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D36" s="15">
+        <v>0</v>
+      </c>
+      <c r="E36" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F36" s="15">
+        <v>0</v>
+      </c>
+      <c r="G36" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H36" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I36" s="15">
+        <v>0</v>
+      </c>
+      <c r="J36" s="15">
+        <v>0</v>
+      </c>
+      <c r="K36" s="15">
+        <v>0</v>
+      </c>
+      <c r="L36" s="15">
+        <v>0</v>
+      </c>
+      <c r="M36" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" s="15">
+        <v>2050</v>
+      </c>
+      <c r="B37" s="15">
+        <v>0</v>
+      </c>
+      <c r="C37" s="15">
+        <v>1.3902642E-4</v>
+      </c>
+      <c r="D37" s="15">
+        <v>0</v>
+      </c>
+      <c r="E37" s="15">
+        <v>3.0122391000000004E-4</v>
+      </c>
+      <c r="F37" s="15">
+        <v>0</v>
+      </c>
+      <c r="G37" s="15">
+        <v>1.2744088500000002E-2</v>
+      </c>
+      <c r="H37" s="15">
+        <v>1.0658692200000001E-3</v>
+      </c>
+      <c r="I37" s="15">
+        <v>0</v>
+      </c>
+      <c r="J37" s="15">
+        <v>0</v>
+      </c>
+      <c r="K37" s="15">
+        <v>0</v>
+      </c>
+      <c r="L37" s="15">
+        <v>0</v>
+      </c>
+      <c r="M37" s="15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8472,12 +9976,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="16384" width="9.1328125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -8518,7 +10022,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="15">
         <v>2015</v>
       </c>
@@ -8559,7 +10063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="15">
         <v>2016</v>
       </c>
@@ -8600,7 +10104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>2017</v>
       </c>
@@ -8641,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="15">
         <v>2018</v>
       </c>
@@ -8682,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="15">
         <v>2019</v>
       </c>
@@ -8723,7 +10227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="15">
         <v>2020</v>
       </c>
@@ -8764,7 +10268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>2021</v>
       </c>
@@ -8805,7 +10309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15">
         <v>2022</v>
       </c>
@@ -8846,7 +10350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>2023</v>
       </c>
@@ -8887,7 +10391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>2024</v>
       </c>
@@ -8928,7 +10432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>2025</v>
       </c>
@@ -8969,7 +10473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>2026</v>
       </c>
@@ -9010,7 +10514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>2027</v>
       </c>
@@ -9051,7 +10555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>2028</v>
       </c>
@@ -9092,7 +10596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>2029</v>
       </c>
@@ -9133,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>2030</v>
       </c>
@@ -9174,7 +10678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>2031</v>
       </c>
@@ -9215,7 +10719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>2032</v>
       </c>
@@ -9256,7 +10760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15">
         <v>2033</v>
       </c>
@@ -9297,7 +10801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15">
         <v>2034</v>
       </c>
@@ -9338,7 +10842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="15">
         <v>2035</v>
       </c>
@@ -9379,7 +10883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15">
         <v>2036</v>
       </c>
@@ -9420,7 +10924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15">
         <v>2037</v>
       </c>
@@ -9461,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="15">
         <v>2038</v>
       </c>
@@ -9502,7 +11006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15">
         <v>2039</v>
       </c>
@@ -9543,7 +11047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15">
         <v>2040</v>
       </c>
@@ -9584,7 +11088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15">
         <v>2041</v>
       </c>
@@ -9625,7 +11129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15">
         <v>2042</v>
       </c>
@@ -9666,7 +11170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15">
         <v>2043</v>
       </c>
@@ -9707,7 +11211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15">
         <v>2044</v>
       </c>
@@ -9748,7 +11252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="15">
         <v>2045</v>
       </c>
@@ -9789,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15">
         <v>2046</v>
       </c>
@@ -9830,7 +11334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15">
         <v>2047</v>
       </c>
@@ -9871,7 +11375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15">
         <v>2048</v>
       </c>
@@ -9912,7 +11416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15">
         <v>2049</v>
       </c>
@@ -9953,7 +11457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15">
         <v>2050</v>
       </c>
@@ -9999,8 +11503,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10010,12 +11514,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="16384" width="9.1328125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -10056,7 +11560,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="15">
         <v>2015</v>
       </c>
@@ -10097,7 +11601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="15">
         <v>2016</v>
       </c>
@@ -10138,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>2017</v>
       </c>
@@ -10179,7 +11683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="15">
         <v>2018</v>
       </c>
@@ -10220,7 +11724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="15">
         <v>2019</v>
       </c>
@@ -10261,7 +11765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="15">
         <v>2020</v>
       </c>
@@ -10302,7 +11806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>2021</v>
       </c>
@@ -10343,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15">
         <v>2022</v>
       </c>
@@ -10384,7 +11888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>2023</v>
       </c>
@@ -10425,7 +11929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>2024</v>
       </c>
@@ -10466,7 +11970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>2025</v>
       </c>
@@ -10507,7 +12011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>2026</v>
       </c>
@@ -10548,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>2027</v>
       </c>
@@ -10589,7 +12093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>2028</v>
       </c>
@@ -10630,7 +12134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>2029</v>
       </c>
@@ -10671,7 +12175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>2030</v>
       </c>
@@ -10712,7 +12216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>2031</v>
       </c>
@@ -10753,7 +12257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>2032</v>
       </c>
@@ -10794,7 +12298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15">
         <v>2033</v>
       </c>
@@ -10835,7 +12339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15">
         <v>2034</v>
       </c>
@@ -10876,7 +12380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="15">
         <v>2035</v>
       </c>
@@ -10917,7 +12421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15">
         <v>2036</v>
       </c>
@@ -10958,7 +12462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15">
         <v>2037</v>
       </c>
@@ -10999,7 +12503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="15">
         <v>2038</v>
       </c>
@@ -11040,7 +12544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15">
         <v>2039</v>
       </c>
@@ -11081,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15">
         <v>2040</v>
       </c>
@@ -11122,7 +12626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15">
         <v>2041</v>
       </c>
@@ -11163,7 +12667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15">
         <v>2042</v>
       </c>
@@ -11204,7 +12708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15">
         <v>2043</v>
       </c>
@@ -11245,7 +12749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15">
         <v>2044</v>
       </c>
@@ -11286,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="15">
         <v>2045</v>
       </c>
@@ -11327,7 +12831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15">
         <v>2046</v>
       </c>
@@ -11368,7 +12872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15">
         <v>2047</v>
       </c>
@@ -11409,7 +12913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15">
         <v>2048</v>
       </c>
@@ -11450,7 +12954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15">
         <v>2049</v>
       </c>
@@ -11491,7 +12995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15">
         <v>2050</v>
       </c>
@@ -11538,12 +13042,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11781,27 +13285,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40B80F8A-689E-45C2-A7FF-D2EFF64979F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6A3BF07-7ED7-416F-97DE-E942FDD976CB}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25F03554-8174-41E4-BC24-B9C12ECA19FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11817,4 +13309,32 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6A3BF07-7ED7-416F-97DE-E942FDD976CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40B80F8A-689E-45C2-A7FF-D2EFF64979F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>